<commit_message>
Replaced "hour of time" with "hour".
</commit_message>
<xml_diff>
--- a/hwc/src/test/resources/fitnesse/hotel_world_clocks_test_tables.xlsx
+++ b/hwc/src/test/resources/fitnesse/hotel_world_clocks_test_tables.xlsx
@@ -57,10 +57,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>to be the correct hour of time</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Check</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -104,6 +100,10 @@
   </si>
   <si>
     <t>due to the end of DST to be</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>to be the correct hour</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -456,8 +456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection sqref="A1:E32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -475,7 +475,7 @@
     </row>
     <row r="2" spans="1:5" ht="40.5" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -500,7 +500,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
@@ -508,7 +508,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
@@ -516,7 +516,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
@@ -524,7 +524,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
@@ -532,7 +532,7 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
         <v>8</v>
@@ -546,7 +546,7 @@
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="D12">
         <v>9</v>
@@ -554,16 +554,16 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" t="s">
         <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E13">
         <v>9</v>
@@ -571,16 +571,16 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E14">
         <v>2</v>
@@ -588,16 +588,16 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C15" t="s">
         <v>7</v>
       </c>
       <c r="D15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E15">
         <v>5</v>
@@ -605,16 +605,16 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C16" t="s">
         <v>8</v>
       </c>
       <c r="D16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E16">
         <v>11</v>
@@ -622,16 +622,16 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C17" t="s">
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E17">
         <v>21</v>
@@ -639,7 +639,7 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -652,7 +652,7 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B22" t="s">
         <v>4</v>
@@ -660,7 +660,7 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -668,7 +668,7 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B24" t="s">
         <v>6</v>
@@ -676,7 +676,7 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B25" t="s">
         <v>7</v>
@@ -684,7 +684,7 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B26" t="s">
         <v>8</v>
@@ -692,13 +692,13 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B27" t="s">
         <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D27">
         <v>0</v>
@@ -706,16 +706,16 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B28" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C28" t="s">
         <v>6</v>
       </c>
       <c r="D28" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E28">
         <v>8</v>
@@ -723,16 +723,16 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B29" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C29" t="s">
         <v>4</v>
       </c>
       <c r="D29" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E29">
         <v>0</v>
@@ -740,16 +740,16 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B30" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C30" t="s">
         <v>7</v>
       </c>
       <c r="D30" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E30">
         <v>4</v>
@@ -757,16 +757,16 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B31" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C31" t="s">
         <v>8</v>
       </c>
       <c r="D31" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E31">
         <v>10</v>
@@ -774,16 +774,16 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B32" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C32" t="s">
         <v>5</v>
       </c>
       <c r="D32" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E32">
         <v>20</v>

</xml_diff>